<commit_message>
Added MainMenuPageNavigationTest.java under src/test/resources/testcases
Added below classes under src/main/java/pages
AppliancesPage.java
CamerasPage.java
ComputingPage.java
GamingPage.java
HomeOutdoorPage.java
HomePage.java
PhonesPage.java
SmartTechPage.java
TVAudioPage.java

Modified LoadPageVerifyURLAndLogoTest.java
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\SeleniumNovStart2021\Currys-ByKorau\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\SeleniumNovStart2021\CurrysDemo\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2391AD5F-CB7E-48A4-B903-601310EA0C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBADE5F-CC93-47E7-977C-BEFB0C48A878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loadPageVerifyURLAndLogo" sheetId="1" r:id="rId1"/>
+    <sheet name="pageNavigation" sheetId="3" r:id="rId2"/>
+    <sheet name="pageNavigation (2)" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>browser</t>
   </si>
@@ -37,6 +39,78 @@
   </si>
   <si>
     <t>https://www.currys.co.uk/gbuk/index.html</t>
+  </si>
+  <si>
+    <t>item name</t>
+  </si>
+  <si>
+    <t>page title</t>
+  </si>
+  <si>
+    <t>item title</t>
+  </si>
+  <si>
+    <t>Computing</t>
+  </si>
+  <si>
+    <t>Laptops, Tablets, Desktop PCs, Computing Accessories | Currys</t>
+  </si>
+  <si>
+    <t>Appliances</t>
+  </si>
+  <si>
+    <t>TV &amp; Audio</t>
+  </si>
+  <si>
+    <t>Gaming</t>
+  </si>
+  <si>
+    <t>Cameras</t>
+  </si>
+  <si>
+    <t>Phones</t>
+  </si>
+  <si>
+    <t>Smart Tech</t>
+  </si>
+  <si>
+    <t>Home &amp; Outdoor</t>
+  </si>
+  <si>
+    <t>Household Appliances</t>
+  </si>
+  <si>
+    <t>Kitchen Appliances, Cookers, Washing Machines | Currys</t>
+  </si>
+  <si>
+    <t>TV and Home Entertainment</t>
+  </si>
+  <si>
+    <t>TVs, DVD &amp; Blu Ray, Home Cinema &amp; Gaming | Currys</t>
+  </si>
+  <si>
+    <t>Gaming | Console and PC Gaming | Currys</t>
+  </si>
+  <si>
+    <t>Digital Cameras, DSLR, Camcorders, Accessories | Currys</t>
+  </si>
+  <si>
+    <t>Cameras and camcorders</t>
+  </si>
+  <si>
+    <t>Mobile Phones &amp; Phones Accessories | Currys Mobile</t>
+  </si>
+  <si>
+    <t>Smart Tech - Get the latest Smart Tech online here | Currys</t>
+  </si>
+  <si>
+    <t>Home &amp; Outdoor Accessories | Currys</t>
+  </si>
+  <si>
+    <t>home and outdoor</t>
+  </si>
+  <si>
+    <t>Mobile Phones</t>
   </si>
 </sst>
 </file>
@@ -357,8 +431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -385,4 +459,212 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4056F0EA-431D-4B7A-AC07-FCD658E6D37C}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E45086-50D6-4ED1-BDAF-74664C18407A}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Commiting the testdata excel with updated test data
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\SeleniumNovStart2021\CurrysDemo\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DBADE5F-CC93-47E7-977C-BEFB0C48A878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060AD66B-E62A-4BE2-B48A-97969F6568C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loadPageVerifyURLAndLogo" sheetId="1" r:id="rId1"/>
-    <sheet name="pageNavigation" sheetId="3" r:id="rId2"/>
-    <sheet name="pageNavigation (2)" sheetId="4" r:id="rId3"/>
+    <sheet name="pageNavigation" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
   <si>
     <t>browser</t>
   </si>
@@ -462,11 +461,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4056F0EA-431D-4B7A-AC07-FCD658E6D37C}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E45086-50D6-4ED1-BDAF-74664C18407A}">
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -495,68 +494,6 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E45086-50D6-4ED1-BDAF-74664C18407A}">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">

</xml_diff>

<commit_message>
Added 5 test cases and corresponding classes.
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\SeleniumNovStart2021\CurrysDemo\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060AD66B-E62A-4BE2-B48A-97969F6568C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024B8975-5F06-4299-A39F-4D8A1EC2F91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loadPageVerifyURLAndLogo" sheetId="1" r:id="rId1"/>
     <sheet name="pageNavigation" sheetId="4" r:id="rId2"/>
+    <sheet name="addProductToBasket" sheetId="5" r:id="rId3"/>
+    <sheet name="trackOurOrder" sheetId="7" r:id="rId4"/>
+    <sheet name="searchProduct" sheetId="8" r:id="rId5"/>
+    <sheet name="currysStoreFinder" sheetId="9" r:id="rId6"/>
+    <sheet name="otherCurrysWebsiteNavigation" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
   <si>
     <t>browser</t>
   </si>
@@ -110,16 +115,177 @@
   </si>
   <si>
     <t>Mobile Phones</t>
+  </si>
+  <si>
+    <t>menu name</t>
+  </si>
+  <si>
+    <t>product name</t>
+  </si>
+  <si>
+    <t>Washing machines</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>Kettles</t>
+  </si>
+  <si>
+    <t>Soundbars</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>item brand</t>
+  </si>
+  <si>
+    <t>NSWM 1043C GG UK N 10 kg 1400 Spin Washing Machine - Graphite</t>
+  </si>
+  <si>
+    <t>HOTPOINT</t>
+  </si>
+  <si>
+    <t>L32SBIN16A 2.1 Sound Bar</t>
+  </si>
+  <si>
+    <t>LOGIK</t>
+  </si>
+  <si>
+    <t>product title</t>
+  </si>
+  <si>
+    <t>Sound bars</t>
+  </si>
+  <si>
+    <t>item added to basket success message</t>
+  </si>
+  <si>
+    <t>This item has been added to your basket</t>
+  </si>
+  <si>
+    <t>ESSENTIALS</t>
+  </si>
+  <si>
+    <t>C17JKW17 Jug Kettle - White</t>
+  </si>
+  <si>
+    <t>job or repair ref</t>
+  </si>
+  <si>
+    <t>search by type</t>
+  </si>
+  <si>
+    <t>search by data</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>A689912</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>UER123</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Contact Number</t>
+  </si>
+  <si>
+    <t>Republic of Ireland</t>
+  </si>
+  <si>
+    <t>78128190</t>
+  </si>
+  <si>
+    <t>search data</t>
+  </si>
+  <si>
+    <t>grinder</t>
+  </si>
+  <si>
+    <t>page Title contains</t>
+  </si>
+  <si>
+    <t>town / postcode</t>
+  </si>
+  <si>
+    <t>expected store</t>
+  </si>
+  <si>
+    <t>UB34FF</t>
+  </si>
+  <si>
+    <t>Currys, Hayes</t>
+  </si>
+  <si>
+    <t>Currys, Penzance</t>
+  </si>
+  <si>
+    <t>penzance</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>expected page title</t>
+  </si>
+  <si>
+    <t>expected URL</t>
+  </si>
+  <si>
+    <t>Currys Business</t>
+  </si>
+  <si>
+    <t>Currys Ireland</t>
+  </si>
+  <si>
+    <t>Partmaster</t>
+  </si>
+  <si>
+    <t>mozilla</t>
+  </si>
+  <si>
+    <t>https://business.currys.co.uk/</t>
+  </si>
+  <si>
+    <t>Welcome - Currys Business</t>
+  </si>
+  <si>
+    <t>https://www.currys.ie/ieen/index.html</t>
+  </si>
+  <si>
+    <t>Currys PC World | Laptops, TVs, Washing Machines, Cookers, Smartphones &amp; Lots More</t>
+  </si>
+  <si>
+    <t>https://www.partmaster.co.uk/</t>
+  </si>
+  <si>
+    <t>Appliance Parts &amp; Electrical Accessories for Home Appliances | Currys Partmaster.co.uk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,14 +308,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E45086-50D6-4ED1-BDAF-74664C18407A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -604,4 +774,366 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB37C37-6438-411E-AAEC-3EB1F4177EA7}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206B7487-B5D5-49AC-947E-DC9347F70FF5}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2">
+        <v>8122332</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4180DAED-0241-4EE5-937C-BB5E8B68F227}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FFED74-22AD-4B6D-B65A-34BC02AFEFD1}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891F8B8F-D48B-48BA-8670-E944FA8CA267}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{B9C5CC96-C23F-4279-94F6-6D96FB946D18}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{7D3CB325-5ACC-4851-AF41-B085FEA2FD59}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{91BAB85A-29CE-4FB3-A823-FCEBE6B6F090}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Renamed test cases class name and added comments
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\SeleniumNovStart2021\CurrysDemo\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024B8975-5F06-4299-A39F-4D8A1EC2F91B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F701C460-8DF1-4826-9690-7E4FDE9326D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loadPageVerifyURLAndLogo" sheetId="1" r:id="rId1"/>
-    <sheet name="pageNavigation" sheetId="4" r:id="rId2"/>
-    <sheet name="addProductToBasket" sheetId="5" r:id="rId3"/>
-    <sheet name="trackOurOrder" sheetId="7" r:id="rId4"/>
-    <sheet name="searchProduct" sheetId="8" r:id="rId5"/>
-    <sheet name="currysStoreFinder" sheetId="9" r:id="rId6"/>
-    <sheet name="otherCurrysWebsiteNavigation" sheetId="10" r:id="rId7"/>
+    <sheet name="searchProduct" sheetId="8" r:id="rId2"/>
+    <sheet name="searchInvalidProduct" sheetId="11" r:id="rId3"/>
+    <sheet name="pageNavigation" sheetId="4" r:id="rId4"/>
+    <sheet name="addProductToBasket" sheetId="12" r:id="rId5"/>
+    <sheet name="addProductToBasket1" sheetId="5" r:id="rId6"/>
+    <sheet name="trackYourOrder" sheetId="7" r:id="rId7"/>
+    <sheet name="currysStoreFinder" sheetId="9" r:id="rId8"/>
+    <sheet name="navigateToOtherCurrysWebsites" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
   <si>
     <t>browser</t>
   </si>
   <si>
-    <t>Page Load URL</t>
-  </si>
-  <si>
     <t>chrome</t>
   </si>
   <si>
@@ -249,9 +248,6 @@
     <t>Partmaster</t>
   </si>
   <si>
-    <t>mozilla</t>
-  </si>
-  <si>
     <t>https://business.currys.co.uk/</t>
   </si>
   <si>
@@ -261,13 +257,28 @@
     <t>https://www.currys.ie/ieen/index.html</t>
   </si>
   <si>
-    <t>Currys PC World | Laptops, TVs, Washing Machines, Cookers, Smartphones &amp; Lots More</t>
-  </si>
-  <si>
     <t>https://www.partmaster.co.uk/</t>
   </si>
   <si>
     <t>Appliance Parts &amp; Electrical Accessories for Home Appliances | Currys Partmaster.co.uk</t>
+  </si>
+  <si>
+    <t>Currys | Laptops, TVs, Washing Machines, Cookers, Smartphones &amp; Lots More</t>
+  </si>
+  <si>
+    <t>expected Page Load URL</t>
+  </si>
+  <si>
+    <t>12132323233323232</t>
+  </si>
+  <si>
+    <t>We can't find a match for "12132323233323232"</t>
+  </si>
+  <si>
+    <t>SAMSUNG</t>
+  </si>
+  <si>
+    <t>Series 5+ Auto Dose WW10T534DAW/S1 WiFi-enabled 10.5 kg 1400 Spin Washing Machine - White</t>
   </si>
 </sst>
 </file>
@@ -314,9 +325,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -601,12 +612,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="37.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -614,15 +625,59 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{53B7145C-1F61-4684-8A3B-402569D733ED}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4180DAED-0241-4EE5-937C-BB5E8B68F227}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -630,12 +685,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A47D227-2BEF-4CF2-964A-200DC5CA82EA}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9E45086-50D6-4ED1-BDAF-74664C18407A}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -650,125 +747,125 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -776,12 +873,127 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB37C37-6438-411E-AAEC-3EB1F4177EA7}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4DD3836-0FE1-420E-9765-6EC6BAD9D5EC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB37C37-6438-411E-AAEC-3EB1F4177EA7}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -799,91 +1011,45 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -891,12 +1057,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206B7487-B5D5-49AC-947E-DC9347F70FF5}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -912,50 +1078,50 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8122332</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="2">
-        <v>8122332</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -964,48 +1130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4180DAED-0241-4EE5-937C-BB5E8B68F227}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FFED74-22AD-4B6D-B65A-34BC02AFEFD1}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1024,32 +1149,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
         <v>60</v>
-      </c>
-      <c r="C1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
         <v>62</v>
-      </c>
-      <c r="C3" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1057,19 +1182,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891F8B8F-D48B-48BA-8670-E944FA8CA267}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="74.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -1077,55 +1202,55 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
         <v>66</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>67</v>
-      </c>
-      <c r="D1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>75</v>
+      <c r="D3" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated project name, added test cases sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\SeleniumNovStart2021\CurrysDemo\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F701C460-8DF1-4826-9690-7E4FDE9326D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E0C2A4-7FCA-4FBD-8FF6-A58A77489B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loadPageVerifyURLAndLogo" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,9 @@
     <sheet name="searchInvalidProduct" sheetId="11" r:id="rId3"/>
     <sheet name="pageNavigation" sheetId="4" r:id="rId4"/>
     <sheet name="addProductToBasket" sheetId="12" r:id="rId5"/>
-    <sheet name="addProductToBasket1" sheetId="5" r:id="rId6"/>
-    <sheet name="trackYourOrder" sheetId="7" r:id="rId7"/>
-    <sheet name="currysStoreFinder" sheetId="9" r:id="rId8"/>
-    <sheet name="navigateToOtherCurrysWebsites" sheetId="10" r:id="rId9"/>
+    <sheet name="trackYourOrder" sheetId="7" r:id="rId6"/>
+    <sheet name="currysStoreFinder" sheetId="9" r:id="rId7"/>
+    <sheet name="navigateToOtherCurrysWebsites" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="80">
   <si>
     <t>browser</t>
   </si>
@@ -138,12 +137,6 @@
   </si>
   <si>
     <t>item brand</t>
-  </si>
-  <si>
-    <t>NSWM 1043C GG UK N 10 kg 1400 Spin Washing Machine - Graphite</t>
-  </si>
-  <si>
-    <t>HOTPOINT</t>
   </si>
   <si>
     <t>L32SBIN16A 2.1 Sound Bar</t>
@@ -611,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -625,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -663,10 +656,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
         <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -674,10 +667,10 @@
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -704,10 +697,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
         <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -715,10 +708,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -877,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4DD3836-0FE1-420E-9765-6EC6BAD9D5EC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -902,7 +895,7 @@
         <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E1" t="s">
         <v>34</v>
@@ -911,7 +904,7 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -928,13 +921,13 @@
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -951,13 +944,13 @@
         <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -971,16 +964,16 @@
         <v>32</v>
       </c>
       <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
         <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -989,75 +982,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB37C37-6438-411E-AAEC-3EB1F4177EA7}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{206B7487-B5D5-49AC-947E-DC9347F70FF5}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1078,16 +1002,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>46</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1098,13 +1022,13 @@
         <v>8122332</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1112,16 +1036,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1130,7 +1054,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FFED74-22AD-4B6D-B65A-34BC02AFEFD1}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1149,10 +1073,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1160,10 +1084,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1171,10 +1095,10 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1182,7 +1106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{891F8B8F-D48B-48BA-8670-E944FA8CA267}">
   <dimension ref="A1:D4"/>
   <sheetViews>
@@ -1202,13 +1126,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
         <v>65</v>
-      </c>
-      <c r="C1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1216,13 +1140,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1230,13 +1154,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1244,13 +1168,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>